<commit_message>
release notes and sprint plan
</commit_message>
<xml_diff>
--- a/Project Planning/Sprint 2 Plan.xlsx
+++ b/Project Planning/Sprint 2 Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="690" windowWidth="19260" windowHeight="7230" activeTab="1"/>
+    <workbookView xWindow="960" yWindow="690" windowWidth="19260" windowHeight="7230"/>
   </bookViews>
   <sheets>
     <sheet name="Plan for Sprint" sheetId="1" r:id="rId1"/>
@@ -361,7 +361,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +403,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -628,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -685,6 +693,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -700,17 +727,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -721,19 +742,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,9 +1041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L43"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1086,10 +1097,10 @@
       </c>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="11"/>
       <c r="E2" s="13"/>
       <c r="F2" s="7"/>
@@ -1122,10 +1133,10 @@
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1344,10 +1355,10 @@
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="11"/>
       <c r="E14" s="13"/>
       <c r="F14" s="7"/>
@@ -1449,10 +1460,10 @@
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="11"/>
       <c r="E19" s="13"/>
       <c r="F19" s="7"/>
@@ -1464,7 +1475,7 @@
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -1487,7 +1498,7 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="30"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="10" t="s">
         <v>43</v>
       </c>
@@ -1508,7 +1519,7 @@
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="30"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="10" t="s">
         <v>44</v>
       </c>
@@ -1529,7 +1540,7 @@
       <c r="L22" s="8"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="30"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="10" t="s">
         <v>45</v>
       </c>
@@ -1550,7 +1561,7 @@
       <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="30"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="10" t="s">
         <v>46</v>
       </c>
@@ -1560,7 +1571,7 @@
       <c r="E24" s="12">
         <v>42278</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="43">
         <v>42282</v>
       </c>
       <c r="G24" s="7"/>
@@ -1571,10 +1582,10 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="27"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="11"/>
       <c r="E25" s="13"/>
       <c r="F25" s="7"/>
@@ -1607,10 +1618,10 @@
       <c r="L26" s="8"/>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -1681,7 +1692,7 @@
         <v>42276</v>
       </c>
       <c r="F30" s="12">
-        <v>42279</v>
+        <v>42278</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="12"/>
@@ -1927,7 +1938,8 @@
     <mergeCell ref="B20:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1935,16 +1947,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:F24"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="56.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
@@ -1990,10 +2002,10 @@
       </c>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="29"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="11"/>
       <c r="E2" s="13"/>
       <c r="F2" s="7"/>
@@ -2026,10 +2038,10 @@
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -2248,10 +2260,10 @@
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="11"/>
       <c r="E14" s="13"/>
       <c r="F14" s="7"/>
@@ -2353,10 +2365,10 @@
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="11"/>
       <c r="E19" s="13"/>
       <c r="F19" s="7"/>
@@ -2368,7 +2380,7 @@
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="40" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -2391,7 +2403,7 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="36"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="10" t="s">
         <v>43</v>
       </c>
@@ -2412,7 +2424,7 @@
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="36"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="10" t="s">
         <v>44</v>
       </c>
@@ -2433,7 +2445,7 @@
       <c r="L22" s="8"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="36"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="10" t="s">
         <v>45</v>
       </c>
@@ -2454,17 +2466,17 @@
       <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="37"/>
-      <c r="C24" s="31" t="s">
+      <c r="B24" s="42"/>
+      <c r="C24" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="31">
         <v>42278</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="31">
         <v>42282</v>
       </c>
       <c r="G24" s="7"/>
@@ -2475,10 +2487,10 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="29"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="11"/>
       <c r="E25" s="13"/>
       <c r="F25" s="7"/>
@@ -2515,9 +2527,9 @@
         <v>50</v>
       </c>
       <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -2526,19 +2538,19 @@
       <c r="L27" s="8"/>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="41">
+      <c r="E28" s="31">
         <v>42271</v>
       </c>
-      <c r="F28" s="41">
+      <c r="F28" s="31">
         <v>42275</v>
       </c>
       <c r="G28" s="7"/>
@@ -2549,19 +2561,19 @@
       <c r="L28" s="8"/>
     </row>
     <row r="29" spans="2:12">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="31">
         <v>42276</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F29" s="31">
         <v>42278</v>
       </c>
       <c r="G29" s="7"/>
@@ -2572,19 +2584,19 @@
       <c r="L29" s="8"/>
     </row>
     <row r="30" spans="2:12">
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="31">
         <v>42276</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="31">
         <v>42279</v>
       </c>
       <c r="G30" s="7"/>

</xml_diff>